<commit_message>
complete facility seg view
</commit_message>
<xml_diff>
--- a/media/exported_facility_json_data.xlsx
+++ b/media/exported_facility_json_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BT4"/>
+  <dimension ref="A1:BT6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -795,7 +795,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -806,17 +806,15 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="n">
-        <v>5</v>
-      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2022-08-17T23:21:37.523332Z</t>
+          <t>2022-08-27T17:46:58.290699Z</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2022-08-25T21:25:20.351754Z</t>
+          <t>2022-08-27T17:46:58.290744Z</t>
         </is>
       </c>
       <c r="K2" t="inlineStr"/>
@@ -901,30 +899,28 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>central ssstore</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>abc0100002</t>
-        </is>
-      </c>
+          <t>test1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>7</v>
+      </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2022-08-17T23:23:27.262880Z</t>
+          <t>2022-08-27T17:47:47.062414Z</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2022-08-25T21:25:32.470766Z</t>
+          <t>2022-08-29T22:25:59.011370Z</t>
         </is>
       </c>
       <c r="K3" t="inlineStr"/>
@@ -999,12 +995,12 @@
       </c>
       <c r="BS3" t="inlineStr">
         <is>
-          <t>sa</t>
+          <t>0</t>
         </is>
       </c>
       <c r="BT3" t="inlineStr">
         <is>
-          <t>mohamad</t>
+          <t>test3</t>
         </is>
       </c>
     </row>
@@ -1013,26 +1009,28 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>sjhlk</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2022-08-25T07:14:22.939851Z</t>
+          <t>2022-08-27T17:48:10.571237Z</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2022-08-25T21:25:40.084280Z</t>
+          <t>2022-08-29T22:25:52.385998Z</t>
         </is>
       </c>
       <c r="K4" t="inlineStr"/>
@@ -1102,15 +1100,233 @@
       </c>
       <c r="BR4" t="inlineStr">
         <is>
-          <t>central ssstore</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="BS4" t="inlineStr">
         <is>
-          <t>sa</t>
+          <t>sadda</t>
         </is>
       </c>
       <c r="BT4" t="inlineStr">
+        <is>
+          <t>test2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>11</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>test3</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2022-08-27T17:51:40.745322Z</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2022-08-29T22:25:45.884907Z</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="b">
+        <v>0</v>
+      </c>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="inlineStr"/>
+      <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="inlineStr"/>
+      <c r="AO5" t="inlineStr"/>
+      <c r="AP5" t="inlineStr"/>
+      <c r="AQ5" t="inlineStr"/>
+      <c r="AR5" t="inlineStr"/>
+      <c r="AS5" t="inlineStr"/>
+      <c r="AT5" t="inlineStr"/>
+      <c r="AU5" t="inlineStr"/>
+      <c r="AV5" t="inlineStr"/>
+      <c r="AW5" t="inlineStr"/>
+      <c r="AX5" t="inlineStr"/>
+      <c r="AY5" t="inlineStr"/>
+      <c r="AZ5" t="inlineStr"/>
+      <c r="BA5" t="inlineStr"/>
+      <c r="BB5" t="inlineStr"/>
+      <c r="BC5" t="inlineStr"/>
+      <c r="BD5" t="inlineStr"/>
+      <c r="BE5" t="inlineStr"/>
+      <c r="BF5" t="inlineStr"/>
+      <c r="BG5" t="inlineStr"/>
+      <c r="BH5" t="inlineStr"/>
+      <c r="BI5" t="inlineStr"/>
+      <c r="BJ5" t="inlineStr"/>
+      <c r="BK5" t="inlineStr"/>
+      <c r="BL5" t="inlineStr"/>
+      <c r="BM5" t="inlineStr"/>
+      <c r="BN5" t="inlineStr"/>
+      <c r="BO5" t="inlineStr"/>
+      <c r="BP5" t="inlineStr"/>
+      <c r="BQ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR5" t="inlineStr">
+        <is>
+          <t>test2</t>
+        </is>
+      </c>
+      <c r="BS5" t="inlineStr">
+        <is>
+          <t>asdad</t>
+        </is>
+      </c>
+      <c r="BT5" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>12</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>mamad</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2022-08-27T17:58:21.421881Z</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>2022-08-29T22:25:37.756867Z</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="b">
+        <v>0</v>
+      </c>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="inlineStr"/>
+      <c r="AI6" t="inlineStr"/>
+      <c r="AJ6" t="inlineStr"/>
+      <c r="AK6" t="inlineStr"/>
+      <c r="AL6" t="inlineStr"/>
+      <c r="AM6" t="inlineStr"/>
+      <c r="AN6" t="inlineStr"/>
+      <c r="AO6" t="inlineStr"/>
+      <c r="AP6" t="inlineStr"/>
+      <c r="AQ6" t="inlineStr"/>
+      <c r="AR6" t="inlineStr"/>
+      <c r="AS6" t="inlineStr"/>
+      <c r="AT6" t="inlineStr"/>
+      <c r="AU6" t="inlineStr"/>
+      <c r="AV6" t="inlineStr"/>
+      <c r="AW6" t="inlineStr"/>
+      <c r="AX6" t="inlineStr"/>
+      <c r="AY6" t="inlineStr"/>
+      <c r="AZ6" t="inlineStr"/>
+      <c r="BA6" t="inlineStr"/>
+      <c r="BB6" t="inlineStr"/>
+      <c r="BC6" t="inlineStr"/>
+      <c r="BD6" t="inlineStr"/>
+      <c r="BE6" t="inlineStr"/>
+      <c r="BF6" t="inlineStr"/>
+      <c r="BG6" t="inlineStr"/>
+      <c r="BH6" t="inlineStr"/>
+      <c r="BI6" t="inlineStr"/>
+      <c r="BJ6" t="inlineStr"/>
+      <c r="BK6" t="inlineStr"/>
+      <c r="BL6" t="inlineStr"/>
+      <c r="BM6" t="inlineStr"/>
+      <c r="BN6" t="inlineStr"/>
+      <c r="BO6" t="inlineStr"/>
+      <c r="BP6" t="inlineStr"/>
+      <c r="BQ6" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR6" t="inlineStr">
+        <is>
+          <t>test3</t>
+        </is>
+      </c>
+      <c r="BS6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BT6" t="inlineStr">
         <is>
           <t>admin</t>
         </is>

</xml_diff>